<commit_message>
Tables for diversity and PERMANOVAs added.
</commit_message>
<xml_diff>
--- a/Tables/Adonis_stats_formatted_table.xlsx
+++ b/Tables/Adonis_stats_formatted_table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/liberjul_msu_edu/Documents/Documents/MSU/Undergrad/Fall 2018/PLP 847/miseq_dat/Leaf_litter_communities/Stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\OneDrive - Michigan State University\Documents\MSU\Undergrad\Fall 2018\PLP 847\miseq_dat\Leaf_litter_communities\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57774640-36A5-41A8-8A51-B79B3EE2846C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{57774640-36A5-41A8-8A51-B79B3EE2846C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A6B73185-F1A2-42C4-B3D0-80A0C04E9C46}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2FBB005A-EE46-46DB-8085-94EA17D58E06}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FBB005A-EE46-46DB-8085-94EA17D58E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Factor</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Endophytes</t>
+  </si>
+  <si>
+    <t>Epiphytes</t>
+  </si>
+  <si>
+    <t>Litter</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Soil</t>
+  </si>
+  <si>
+    <t>All-factor PERMANOVA test statistics</t>
+  </si>
+  <si>
+    <t>Pairwise PERMANOVA comparisons by substrate</t>
   </si>
 </sst>
 </file>
@@ -204,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -244,6 +265,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,156 +586,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D20280-0AAB-448F-9018-F36E94EE6D76}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="F1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B3" s="5">
         <v>0.30790000000000001</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="5">
         <v>19.62</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D3" s="6">
         <v>1E-3</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B4" s="8">
         <v>7.51E-2</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C4" s="8">
         <v>14.37</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D4" s="9">
         <v>1E-3</v>
       </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B5" s="5">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="5">
         <v>4.13</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="6">
         <v>1E-3</v>
       </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>1.5E-3</v>
+      </c>
+      <c r="H5">
+        <v>1.5E-3</v>
+      </c>
+      <c r="I5">
+        <v>1.5E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B6" s="8">
         <v>0.1057</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C6" s="8">
         <v>6.74</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D6" s="9">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B7" s="5">
         <v>0.20630000000000001</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="5">
         <v>3.29</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D7" s="6">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B8" s="8">
         <v>5.5100000000000003E-2</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C8" s="8">
         <v>2.63</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D8" s="9">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B9" s="5">
         <v>0.1216</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="5">
         <v>2.3199999999999998</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="6">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="7" t="s">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B10" s="8">
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AFDA51084187F242B05EFA296C5963FF" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3643f2840fd34a552c287b84deed346">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3ea71f81-dc8a-4f4b-b0dd-c828e930e924" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bc954b55e77a02dd874654cc5b225bc" ns3:_="">
     <xsd:import namespace="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
@@ -892,22 +1000,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5415DCD-4D3A-44BB-A3D8-2DEFAFE826EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B62996BE-13F2-4E92-87C5-9001C2C494E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAEC7F55-0486-4602-9A8E-2E5694DC4C07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -923,28 +1040,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B62996BE-13F2-4E92-87C5-9001C2C494E6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5415DCD-4D3A-44BB-A3D8-2DEFAFE826EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Table formatting and label changes.
</commit_message>
<xml_diff>
--- a/Tables/Adonis_stats_formatted_table.xlsx
+++ b/Tables/Adonis_stats_formatted_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\OneDrive - Michigan State University\Documents\MSU\Undergrad\Fall 2018\PLP 847\miseq_dat\Leaf_litter_communities\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{57774640-36A5-41A8-8A51-B79B3EE2846C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A6B73185-F1A2-42C4-B3D0-80A0C04E9C46}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{57774640-36A5-41A8-8A51-B79B3EE2846C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{95849DE4-A6A2-4BC2-B5AF-9EC6C503BD5B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2FBB005A-EE46-46DB-8085-94EA17D58E06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2FBB005A-EE46-46DB-8085-94EA17D58E06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Substrate</t>
   </si>
   <si>
-    <t>Plant species</t>
-  </si>
-  <si>
     <t>Site</t>
   </si>
   <si>
@@ -91,13 +88,16 @@
   </si>
   <si>
     <t>Pairwise PERMANOVA comparisons by substrate</t>
+  </si>
+  <si>
+    <t>Host species</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,47 +105,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFDA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -153,123 +122,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA9D08E"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFA9D08E"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFA9D08E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFA9D08E"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFA9D08E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFA9D08E"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA9D08E"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFA9D08E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFA9D08E"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA9D08E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA9D08E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFA9D08E"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA9D08E"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -586,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D20280-0AAB-448F-9018-F36E94EE6D76}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,201 +459,203 @@
     <col min="9" max="9" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.30790000000000001</v>
+      </c>
+      <c r="C3">
+        <v>19.62</v>
+      </c>
+      <c r="D3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>7.51E-2</v>
+      </c>
+      <c r="C4">
+        <v>14.37</v>
+      </c>
+      <c r="D4">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>8.6400000000000005E-2</v>
+      </c>
+      <c r="C5">
+        <v>4.13</v>
+      </c>
+      <c r="D5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.1057</v>
+      </c>
+      <c r="C6">
+        <v>6.74</v>
+      </c>
+      <c r="D6">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.20630000000000001</v>
+      </c>
+      <c r="C7">
+        <v>3.29</v>
+      </c>
+      <c r="D7">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>5.5100000000000003E-2</v>
+      </c>
+      <c r="C8">
+        <v>2.63</v>
+      </c>
+      <c r="D8">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.1216</v>
+      </c>
+      <c r="C9">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D9">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>4.1799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="F1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0.30790000000000001</v>
-      </c>
-      <c r="C3" s="5">
-        <v>19.62</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="G3">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="B16">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C16">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="8">
-        <v>7.51E-2</v>
-      </c>
-      <c r="C4" s="8">
-        <v>14.37</v>
-      </c>
-      <c r="D4" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="H4">
+      <c r="B17">
         <v>1.5E-3</v>
       </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5">
-        <v>8.6400000000000005E-2</v>
-      </c>
-      <c r="C5" s="5">
-        <v>4.13</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1E-3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5">
+      <c r="C17">
         <v>1.5E-3</v>
       </c>
-      <c r="H5">
+      <c r="D17">
         <v>1.5E-3</v>
       </c>
-      <c r="I5">
-        <v>1.5E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.1057</v>
-      </c>
-      <c r="C6" s="8">
-        <v>6.74</v>
-      </c>
-      <c r="D6" s="9">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5">
-        <v>0.20630000000000001</v>
-      </c>
-      <c r="C7" s="5">
-        <v>3.29</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="8">
-        <v>5.5100000000000003E-2</v>
-      </c>
-      <c r="C8" s="8">
-        <v>2.63</v>
-      </c>
-      <c r="D8" s="9">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0.1216</v>
-      </c>
-      <c r="C9" s="5">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="8">
-        <v>4.1799999999999997E-2</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -808,15 +669,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AFDA51084187F242B05EFA296C5963FF" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3643f2840fd34a552c287b84deed346">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3ea71f81-dc8a-4f4b-b0dd-c828e930e924" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bc954b55e77a02dd874654cc5b225bc" ns3:_="">
     <xsd:import namespace="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
@@ -1000,16 +852,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5415DCD-4D3A-44BB-A3D8-2DEFAFE826EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3ea71f81-dc8a-4f4b-b0dd-c828e930e924"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
@@ -1017,14 +878,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B62996BE-13F2-4E92-87C5-9001C2C494E6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAEC7F55-0486-4602-9A8E-2E5694DC4C07}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1040,4 +893,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B62996BE-13F2-4E92-87C5-9001C2C494E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>